<commit_message>
Adding v0.0.1 and v0.0.2 folders
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas\Desktop\ffn\m2\thesis\nf_reqextractor\git\nf_reqextractor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A10596-EE2F-4585-A54D-908000C55200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5FC2E49-F651-468B-832B-8500D1E458E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{EC085558-F660-44D9-8D61-E2A64C91A3B9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="48">
   <si>
     <t>loss</t>
   </si>
@@ -165,13 +165,28 @@
   </si>
   <si>
     <t>average percentage of success on the prediction of all tests</t>
+  </si>
+  <si>
+    <t>occurrence of categories of software requirements and specifications dataset (requirements_v0_0_1.csv)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>main_v0_0_1</t>
+  </si>
+  <si>
+    <t>main_v0_0_2</t>
+  </si>
+  <si>
+    <t>TOTAL /16</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,8 +217,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -240,8 +263,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="36">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -695,6 +730,26 @@
         <color indexed="64"/>
       </left>
       <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -702,13 +757,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -718,7 +771,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -726,8 +779,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -803,8 +854,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -851,20 +900,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -901,7 +942,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -910,7 +951,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -921,6 +962,80 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1236,10 +1351,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEE16F68-CDB6-4331-8858-0654CB9651F9}">
-  <dimension ref="A1:R19"/>
+  <dimension ref="A1:R38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1261,297 +1376,299 @@
     <col min="15" max="15" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.140625" style="32" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.140625" style="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="30"/>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="70" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
-      <c r="J1" s="71"/>
-      <c r="K1" s="71"/>
-      <c r="L1" s="71"/>
-      <c r="M1" s="71"/>
-      <c r="N1" s="71"/>
-      <c r="O1" s="71"/>
-      <c r="P1" s="71"/>
-      <c r="Q1" s="72"/>
-      <c r="R1" s="53"/>
+      <c r="A1" s="77" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="62" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
+      <c r="O1" s="63"/>
+      <c r="P1" s="63"/>
+      <c r="Q1" s="64"/>
+      <c r="R1" s="75"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="15" t="s">
+      <c r="A2" s="77"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="I2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="J2" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="K2" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="L2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="16" t="s">
+      <c r="M2" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="N2" s="17" t="s">
+      <c r="N2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="16" t="s">
+      <c r="O2" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="P2" s="17" t="s">
+      <c r="P2" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="Q2" s="18" t="s">
+      <c r="Q2" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="R2" s="54" t="s">
+      <c r="R2" s="46" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="30"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="5">
+      <c r="A3" s="77"/>
+      <c r="B3" s="77"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="3">
         <v>255</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="5">
         <v>21</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="4">
         <v>10</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="5">
         <v>13</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="4">
         <v>38</v>
       </c>
-      <c r="K3" s="7">
+      <c r="K3" s="5">
         <v>17</v>
       </c>
-      <c r="L3" s="6">
+      <c r="L3" s="4">
         <v>62</v>
       </c>
-      <c r="M3" s="7">
+      <c r="M3" s="5">
         <v>54</v>
       </c>
-      <c r="N3" s="6">
-        <v>1</v>
-      </c>
-      <c r="O3" s="7">
+      <c r="N3" s="4">
+        <v>1</v>
+      </c>
+      <c r="O3" s="5">
         <v>21</v>
       </c>
-      <c r="P3" s="6">
+      <c r="P3" s="4">
         <v>66</v>
       </c>
-      <c r="Q3" s="8">
+      <c r="Q3" s="6">
         <v>67</v>
       </c>
-      <c r="R3" s="50">
+      <c r="R3" s="45">
         <f>SUM(F3:Q3)</f>
         <v>625</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="30"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="30"/>
-      <c r="Q4" s="30"/>
-      <c r="R4" s="31"/>
+      <c r="A4" s="79"/>
+      <c r="B4" s="79"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="72"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="73"/>
+      <c r="L4" s="73"/>
+      <c r="M4" s="73"/>
+      <c r="N4" s="73"/>
+      <c r="O4" s="73"/>
+      <c r="P4" s="71"/>
+      <c r="Q4" s="71"/>
+      <c r="R4" s="74"/>
     </row>
     <row r="5" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="70" t="s">
+      <c r="A5" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="71"/>
-      <c r="C5" s="72"/>
-      <c r="D5" s="70" t="s">
+      <c r="B5" s="63"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="62" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="72"/>
-      <c r="F5" s="70" t="s">
+      <c r="E5" s="64"/>
+      <c r="F5" s="62" t="s">
         <v>38</v>
       </c>
-      <c r="G5" s="71"/>
-      <c r="H5" s="71"/>
-      <c r="I5" s="71"/>
-      <c r="J5" s="71"/>
-      <c r="K5" s="71"/>
-      <c r="L5" s="71"/>
-      <c r="M5" s="71"/>
-      <c r="N5" s="71"/>
-      <c r="O5" s="71"/>
-      <c r="P5" s="71"/>
-      <c r="Q5" s="71"/>
-      <c r="R5" s="72"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="63"/>
+      <c r="I5" s="63"/>
+      <c r="J5" s="63"/>
+      <c r="K5" s="63"/>
+      <c r="L5" s="63"/>
+      <c r="M5" s="63"/>
+      <c r="N5" s="63"/>
+      <c r="O5" s="63"/>
+      <c r="P5" s="63"/>
+      <c r="Q5" s="63"/>
+      <c r="R5" s="64"/>
     </row>
     <row r="6" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="35" t="s">
+      <c r="A6" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="34" t="s">
+      <c r="D6" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="36" t="s">
+      <c r="E6" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="37" t="s">
+      <c r="F6" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="38" t="s">
+      <c r="G6" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="39" t="s">
+      <c r="H6" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="38" t="s">
+      <c r="I6" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="J6" s="39" t="s">
+      <c r="J6" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="38" t="s">
+      <c r="K6" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="L6" s="39" t="s">
+      <c r="L6" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="M6" s="38" t="s">
+      <c r="M6" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="N6" s="39" t="s">
+      <c r="N6" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="O6" s="38" t="s">
+      <c r="O6" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="P6" s="39" t="s">
+      <c r="P6" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="Q6" s="40" t="s">
+      <c r="Q6" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="R6" s="25" t="s">
+      <c r="R6" s="23" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="43" t="s">
+      <c r="C7" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="42">
+      <c r="D7" s="38">
         <v>150</v>
       </c>
-      <c r="E7" s="44">
+      <c r="E7" s="40">
         <v>600</v>
       </c>
-      <c r="F7" s="45">
-        <v>1</v>
-      </c>
-      <c r="G7" s="46">
-        <v>1</v>
-      </c>
-      <c r="H7" s="46">
-        <v>0</v>
-      </c>
-      <c r="I7" s="46">
-        <v>1</v>
-      </c>
-      <c r="J7" s="46">
-        <v>1</v>
-      </c>
-      <c r="K7" s="46">
-        <v>0</v>
-      </c>
-      <c r="L7" s="46">
-        <v>0</v>
-      </c>
-      <c r="M7" s="46">
-        <v>1</v>
-      </c>
-      <c r="N7" s="46">
-        <v>0</v>
-      </c>
-      <c r="O7" s="46">
-        <v>0</v>
-      </c>
-      <c r="P7" s="46">
+      <c r="F7" s="41">
+        <v>1</v>
+      </c>
+      <c r="G7" s="42">
+        <v>1</v>
+      </c>
+      <c r="H7" s="42">
+        <v>0</v>
+      </c>
+      <c r="I7" s="42">
+        <v>1</v>
+      </c>
+      <c r="J7" s="42">
+        <v>1</v>
+      </c>
+      <c r="K7" s="42">
+        <v>0</v>
+      </c>
+      <c r="L7" s="42">
+        <v>0</v>
+      </c>
+      <c r="M7" s="42">
+        <v>1</v>
+      </c>
+      <c r="N7" s="42">
+        <v>0</v>
+      </c>
+      <c r="O7" s="42">
+        <v>0</v>
+      </c>
+      <c r="P7" s="42">
         <v>2</v>
       </c>
-      <c r="Q7" s="47">
-        <v>0</v>
-      </c>
-      <c r="R7" s="26">
+      <c r="Q7" s="43">
+        <v>0</v>
+      </c>
+      <c r="R7" s="24">
         <f>(SUM(F7:Q7))</f>
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="8">
         <v>250</v>
       </c>
-      <c r="E8" s="19">
+      <c r="E8" s="17">
         <v>600</v>
       </c>
       <c r="F8" s="2">
@@ -1587,256 +1704,256 @@
       <c r="P8" s="1">
         <v>1</v>
       </c>
-      <c r="Q8" s="23">
-        <v>0</v>
-      </c>
-      <c r="R8" s="27">
+      <c r="Q8" s="21">
+        <v>0</v>
+      </c>
+      <c r="R8" s="25">
         <f t="shared" ref="R8:R14" si="0">(SUM(F8:Q8))</f>
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="11">
         <v>350</v>
       </c>
-      <c r="E9" s="20">
+      <c r="E9" s="18">
         <v>600</v>
       </c>
-      <c r="F9" s="21">
+      <c r="F9" s="19">
         <v>2</v>
       </c>
-      <c r="G9" s="22">
-        <v>0</v>
-      </c>
-      <c r="H9" s="22">
-        <v>0</v>
-      </c>
-      <c r="I9" s="22">
-        <v>0</v>
-      </c>
-      <c r="J9" s="22">
+      <c r="G9" s="20">
+        <v>0</v>
+      </c>
+      <c r="H9" s="20">
+        <v>0</v>
+      </c>
+      <c r="I9" s="20">
+        <v>0</v>
+      </c>
+      <c r="J9" s="20">
         <v>2</v>
       </c>
-      <c r="K9" s="22">
-        <v>0</v>
-      </c>
-      <c r="L9" s="22">
-        <v>0</v>
-      </c>
-      <c r="M9" s="22">
-        <v>1</v>
-      </c>
-      <c r="N9" s="22">
-        <v>0</v>
-      </c>
-      <c r="O9" s="22">
-        <v>0</v>
-      </c>
-      <c r="P9" s="22">
+      <c r="K9" s="20">
+        <v>0</v>
+      </c>
+      <c r="L9" s="20">
+        <v>0</v>
+      </c>
+      <c r="M9" s="20">
+        <v>1</v>
+      </c>
+      <c r="N9" s="20">
+        <v>0</v>
+      </c>
+      <c r="O9" s="20">
+        <v>0</v>
+      </c>
+      <c r="P9" s="20">
         <v>2</v>
       </c>
-      <c r="Q9" s="24">
-        <v>0</v>
-      </c>
-      <c r="R9" s="28">
+      <c r="Q9" s="22">
+        <v>0</v>
+      </c>
+      <c r="R9" s="26">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="63" t="s">
+      <c r="A10" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="64" t="s">
+      <c r="B10" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="65" t="s">
+      <c r="C10" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="64">
+      <c r="D10" s="56">
         <v>150</v>
       </c>
-      <c r="E10" s="66">
+      <c r="E10" s="58">
         <v>600</v>
       </c>
-      <c r="F10" s="67">
+      <c r="F10" s="59">
         <v>2</v>
       </c>
-      <c r="G10" s="68">
-        <v>0</v>
-      </c>
-      <c r="H10" s="68">
-        <v>0</v>
-      </c>
-      <c r="I10" s="68">
-        <v>0</v>
-      </c>
-      <c r="J10" s="68">
-        <v>0</v>
-      </c>
-      <c r="K10" s="68">
-        <v>0</v>
-      </c>
-      <c r="L10" s="68">
-        <v>0</v>
-      </c>
-      <c r="M10" s="68">
-        <v>0</v>
-      </c>
-      <c r="N10" s="68">
-        <v>0</v>
-      </c>
-      <c r="O10" s="68">
-        <v>0</v>
-      </c>
-      <c r="P10" s="68">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="69">
-        <v>0</v>
-      </c>
-      <c r="R10" s="29">
+      <c r="G10" s="60">
+        <v>0</v>
+      </c>
+      <c r="H10" s="60">
+        <v>0</v>
+      </c>
+      <c r="I10" s="60">
+        <v>0</v>
+      </c>
+      <c r="J10" s="60">
+        <v>0</v>
+      </c>
+      <c r="K10" s="60">
+        <v>0</v>
+      </c>
+      <c r="L10" s="60">
+        <v>0</v>
+      </c>
+      <c r="M10" s="60">
+        <v>0</v>
+      </c>
+      <c r="N10" s="60">
+        <v>0</v>
+      </c>
+      <c r="O10" s="60">
+        <v>0</v>
+      </c>
+      <c r="P10" s="60">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="61">
+        <v>0</v>
+      </c>
+      <c r="R10" s="27">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="55" t="s">
+      <c r="A11" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="56" t="s">
+      <c r="B11" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="57" t="s">
+      <c r="C11" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="56">
+      <c r="D11" s="48">
         <v>250</v>
       </c>
-      <c r="E11" s="58">
+      <c r="E11" s="50">
         <v>600</v>
       </c>
-      <c r="F11" s="59">
+      <c r="F11" s="51">
         <v>2</v>
       </c>
-      <c r="G11" s="60">
-        <v>0</v>
-      </c>
-      <c r="H11" s="60">
-        <v>0</v>
-      </c>
-      <c r="I11" s="60">
-        <v>0</v>
-      </c>
-      <c r="J11" s="60">
-        <v>0</v>
-      </c>
-      <c r="K11" s="60">
-        <v>0</v>
-      </c>
-      <c r="L11" s="60">
-        <v>0</v>
-      </c>
-      <c r="M11" s="60">
-        <v>0</v>
-      </c>
-      <c r="N11" s="60">
-        <v>0</v>
-      </c>
-      <c r="O11" s="60">
-        <v>0</v>
-      </c>
-      <c r="P11" s="60">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="61">
-        <v>0</v>
-      </c>
-      <c r="R11" s="62">
+      <c r="G11" s="52">
+        <v>0</v>
+      </c>
+      <c r="H11" s="52">
+        <v>0</v>
+      </c>
+      <c r="I11" s="52">
+        <v>0</v>
+      </c>
+      <c r="J11" s="52">
+        <v>0</v>
+      </c>
+      <c r="K11" s="52">
+        <v>0</v>
+      </c>
+      <c r="L11" s="52">
+        <v>0</v>
+      </c>
+      <c r="M11" s="52">
+        <v>0</v>
+      </c>
+      <c r="N11" s="52">
+        <v>0</v>
+      </c>
+      <c r="O11" s="52">
+        <v>0</v>
+      </c>
+      <c r="P11" s="52">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="53">
+        <v>0</v>
+      </c>
+      <c r="R11" s="54">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="43" t="s">
+      <c r="C12" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="42">
+      <c r="D12" s="38">
         <v>100</v>
       </c>
-      <c r="E12" s="43">
+      <c r="E12" s="39">
         <v>600</v>
       </c>
-      <c r="F12" s="46">
-        <v>1</v>
-      </c>
-      <c r="G12" s="46">
-        <v>1</v>
-      </c>
-      <c r="H12" s="46">
-        <v>0</v>
-      </c>
-      <c r="I12" s="46">
-        <v>0</v>
-      </c>
-      <c r="J12" s="46">
+      <c r="F12" s="42">
+        <v>1</v>
+      </c>
+      <c r="G12" s="42">
+        <v>1</v>
+      </c>
+      <c r="H12" s="42">
+        <v>0</v>
+      </c>
+      <c r="I12" s="42">
+        <v>0</v>
+      </c>
+      <c r="J12" s="42">
         <v>2</v>
       </c>
-      <c r="K12" s="46">
-        <v>0</v>
-      </c>
-      <c r="L12" s="46">
-        <v>0</v>
-      </c>
-      <c r="M12" s="46">
-        <v>0</v>
-      </c>
-      <c r="N12" s="46">
-        <v>0</v>
-      </c>
-      <c r="O12" s="46">
-        <v>0</v>
-      </c>
-      <c r="P12" s="46">
+      <c r="K12" s="42">
+        <v>0</v>
+      </c>
+      <c r="L12" s="42">
+        <v>0</v>
+      </c>
+      <c r="M12" s="42">
+        <v>0</v>
+      </c>
+      <c r="N12" s="42">
+        <v>0</v>
+      </c>
+      <c r="O12" s="42">
+        <v>0</v>
+      </c>
+      <c r="P12" s="42">
         <v>2</v>
       </c>
-      <c r="Q12" s="47">
-        <v>0</v>
-      </c>
-      <c r="R12" s="26">
+      <c r="Q12" s="43">
+        <v>0</v>
+      </c>
+      <c r="R12" s="24">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="8">
         <v>150</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="9">
         <v>600</v>
       </c>
       <c r="F13" s="1">
@@ -1872,205 +1989,948 @@
       <c r="P13" s="1">
         <v>2</v>
       </c>
-      <c r="Q13" s="23">
-        <v>1</v>
-      </c>
-      <c r="R13" s="27">
+      <c r="Q13" s="21">
+        <v>1</v>
+      </c>
+      <c r="R13" s="25">
         <f t="shared" ref="R13" si="1">(SUM(F13:Q13))</f>
         <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14" s="11">
         <v>250</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="12">
         <v>600</v>
       </c>
-      <c r="F14" s="22">
+      <c r="F14" s="20">
         <v>2</v>
       </c>
-      <c r="G14" s="22">
-        <v>1</v>
-      </c>
-      <c r="H14" s="22">
-        <v>0</v>
-      </c>
-      <c r="I14" s="22">
-        <v>1</v>
-      </c>
-      <c r="J14" s="22">
+      <c r="G14" s="20">
+        <v>1</v>
+      </c>
+      <c r="H14" s="20">
+        <v>0</v>
+      </c>
+      <c r="I14" s="20">
+        <v>1</v>
+      </c>
+      <c r="J14" s="20">
         <v>2</v>
       </c>
-      <c r="K14" s="22">
-        <v>0</v>
-      </c>
-      <c r="L14" s="22">
-        <v>0</v>
-      </c>
-      <c r="M14" s="22">
-        <v>0</v>
-      </c>
-      <c r="N14" s="22">
-        <v>0</v>
-      </c>
-      <c r="O14" s="22">
-        <v>0</v>
-      </c>
-      <c r="P14" s="22">
+      <c r="K14" s="20">
+        <v>0</v>
+      </c>
+      <c r="L14" s="20">
+        <v>0</v>
+      </c>
+      <c r="M14" s="20">
+        <v>0</v>
+      </c>
+      <c r="N14" s="20">
+        <v>0</v>
+      </c>
+      <c r="O14" s="20">
+        <v>0</v>
+      </c>
+      <c r="P14" s="20">
         <v>2</v>
       </c>
-      <c r="Q14" s="24">
-        <v>1</v>
-      </c>
-      <c r="R14" s="28">
+      <c r="Q14" s="20">
+        <v>1</v>
+      </c>
+      <c r="R14" s="26">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="30"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="30"/>
-      <c r="M15" s="30"/>
-      <c r="N15" s="30"/>
-      <c r="O15" s="30"/>
-      <c r="P15" s="30"/>
-      <c r="Q15" s="48" t="s">
-        <v>21</v>
-      </c>
-      <c r="R15" s="50">
+    <row r="15" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="71"/>
+      <c r="B15" s="71"/>
+      <c r="C15" s="71"/>
+      <c r="D15" s="71"/>
+      <c r="E15" s="71"/>
+      <c r="F15" s="72"/>
+      <c r="G15" s="73"/>
+      <c r="H15" s="73"/>
+      <c r="I15" s="73"/>
+      <c r="J15" s="73"/>
+      <c r="K15" s="73"/>
+      <c r="L15" s="73"/>
+      <c r="M15" s="73"/>
+      <c r="N15" s="73"/>
+      <c r="O15" s="73"/>
+      <c r="P15" s="71"/>
+      <c r="Q15" s="71"/>
+      <c r="R15" s="45">
         <f>AVERAGE(R7:R14)</f>
         <v>6.375</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="30"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="70" t="s">
+      <c r="A16" s="71"/>
+      <c r="B16" s="71"/>
+      <c r="C16" s="71"/>
+      <c r="D16" s="71"/>
+      <c r="E16" s="71"/>
+      <c r="F16" s="62" t="s">
         <v>42</v>
       </c>
-      <c r="G16" s="71"/>
-      <c r="H16" s="71"/>
-      <c r="I16" s="71"/>
-      <c r="J16" s="71"/>
-      <c r="K16" s="71"/>
-      <c r="L16" s="71"/>
-      <c r="M16" s="71"/>
-      <c r="N16" s="71"/>
-      <c r="O16" s="71"/>
-      <c r="P16" s="71"/>
-      <c r="Q16" s="71"/>
-      <c r="R16" s="51"/>
+      <c r="G16" s="63"/>
+      <c r="H16" s="63"/>
+      <c r="I16" s="63"/>
+      <c r="J16" s="63"/>
+      <c r="K16" s="63"/>
+      <c r="L16" s="63"/>
+      <c r="M16" s="63"/>
+      <c r="N16" s="63"/>
+      <c r="O16" s="63"/>
+      <c r="P16" s="63"/>
+      <c r="Q16" s="64"/>
+      <c r="R16" s="76"/>
     </row>
     <row r="17" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="30"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="29">
+      <c r="A17" s="71"/>
+      <c r="B17" s="71"/>
+      <c r="C17" s="71"/>
+      <c r="D17" s="71"/>
+      <c r="E17" s="71"/>
+      <c r="F17" s="27">
         <f t="shared" ref="F17:Q17" si="2">AVERAGE(F7:F14)/2*100</f>
         <v>81.25</v>
       </c>
-      <c r="G17" s="29">
+      <c r="G17" s="27">
         <f t="shared" si="2"/>
         <v>31.25</v>
       </c>
-      <c r="H17" s="29">
+      <c r="H17" s="27">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I17" s="29">
+      <c r="I17" s="27">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="J17" s="29">
+      <c r="J17" s="27">
         <f t="shared" si="2"/>
         <v>68.75</v>
       </c>
-      <c r="K17" s="29">
+      <c r="K17" s="27">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L17" s="29">
+      <c r="L17" s="27">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M17" s="29">
+      <c r="M17" s="27">
         <f t="shared" si="2"/>
         <v>18.75</v>
       </c>
-      <c r="N17" s="29">
+      <c r="N17" s="27">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O17" s="29">
+      <c r="O17" s="27">
         <f t="shared" si="2"/>
         <v>12.5</v>
       </c>
-      <c r="P17" s="29">
+      <c r="P17" s="27">
         <f t="shared" si="2"/>
         <v>68.75</v>
       </c>
-      <c r="Q17" s="49">
+      <c r="Q17" s="44">
         <f t="shared" si="2"/>
         <v>12.5</v>
       </c>
-      <c r="R17" s="50">
+      <c r="R17" s="45">
         <f>SUM(F17:Q17)</f>
         <v>318.75</v>
       </c>
     </row>
     <row r="18" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="30"/>
-      <c r="B18" s="30"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="30"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="30"/>
-      <c r="J18" s="30"/>
-      <c r="K18" s="30"/>
-      <c r="L18" s="30"/>
-      <c r="M18" s="30"/>
-      <c r="N18" s="30"/>
-      <c r="O18" s="30"/>
-      <c r="P18" s="30"/>
-      <c r="Q18" s="30"/>
-      <c r="R18" s="50">
+      <c r="A18" s="71"/>
+      <c r="B18" s="71"/>
+      <c r="C18" s="71"/>
+      <c r="D18" s="71"/>
+      <c r="E18" s="71"/>
+      <c r="F18" s="72"/>
+      <c r="G18" s="73"/>
+      <c r="H18" s="73"/>
+      <c r="I18" s="73"/>
+      <c r="J18" s="73"/>
+      <c r="K18" s="73"/>
+      <c r="L18" s="73"/>
+      <c r="M18" s="73"/>
+      <c r="N18" s="73"/>
+      <c r="O18" s="73"/>
+      <c r="P18" s="71"/>
+      <c r="Q18" s="71"/>
+      <c r="R18" s="45">
         <f>AVERAGE(F17:Q17)</f>
         <v>26.5625</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="R19" s="52"/>
+    <row r="19" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="67" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="67"/>
+      <c r="C19" s="67"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="68"/>
+      <c r="F19" s="62" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" s="63"/>
+      <c r="H19" s="63"/>
+      <c r="I19" s="63"/>
+      <c r="J19" s="63"/>
+      <c r="K19" s="63"/>
+      <c r="L19" s="63"/>
+      <c r="M19" s="63"/>
+      <c r="N19" s="63"/>
+      <c r="O19" s="63"/>
+      <c r="P19" s="63"/>
+      <c r="Q19" s="64"/>
+      <c r="R19" s="73"/>
+    </row>
+    <row r="20" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="67"/>
+      <c r="B20" s="67"/>
+      <c r="C20" s="67"/>
+      <c r="D20" s="67"/>
+      <c r="E20" s="68"/>
+      <c r="F20" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" s="65"/>
+      <c r="I20" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="J20" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="K20" s="65"/>
+      <c r="L20" s="65"/>
+      <c r="M20" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="N20" s="65"/>
+      <c r="O20" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="P20" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q20" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="R20" s="46" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="67"/>
+      <c r="B21" s="67"/>
+      <c r="C21" s="67"/>
+      <c r="D21" s="67"/>
+      <c r="E21" s="68"/>
+      <c r="F21" s="3">
+        <v>255</v>
+      </c>
+      <c r="G21" s="5">
+        <v>21</v>
+      </c>
+      <c r="H21" s="66"/>
+      <c r="I21" s="5">
+        <v>13</v>
+      </c>
+      <c r="J21" s="4">
+        <v>38</v>
+      </c>
+      <c r="K21" s="66"/>
+      <c r="L21" s="66"/>
+      <c r="M21" s="5">
+        <v>54</v>
+      </c>
+      <c r="N21" s="66"/>
+      <c r="O21" s="5">
+        <v>21</v>
+      </c>
+      <c r="P21" s="4">
+        <v>66</v>
+      </c>
+      <c r="Q21" s="6">
+        <v>67</v>
+      </c>
+      <c r="R21" s="45">
+        <f>SUM(F21:Q21)</f>
+        <v>535</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="69"/>
+      <c r="B22" s="69"/>
+      <c r="C22" s="69"/>
+      <c r="D22" s="69"/>
+      <c r="E22" s="70"/>
+      <c r="F22" s="72"/>
+      <c r="G22" s="73"/>
+      <c r="H22" s="73"/>
+      <c r="I22" s="73"/>
+      <c r="J22" s="73"/>
+      <c r="K22" s="73"/>
+      <c r="L22" s="73"/>
+      <c r="M22" s="73"/>
+      <c r="N22" s="73"/>
+      <c r="O22" s="73"/>
+      <c r="P22" s="71"/>
+      <c r="Q22" s="71"/>
+      <c r="R22" s="74"/>
+    </row>
+    <row r="23" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="63"/>
+      <c r="C23" s="64"/>
+      <c r="D23" s="62" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="64"/>
+      <c r="F23" s="62" t="s">
+        <v>38</v>
+      </c>
+      <c r="G23" s="63"/>
+      <c r="H23" s="63"/>
+      <c r="I23" s="63"/>
+      <c r="J23" s="63"/>
+      <c r="K23" s="63"/>
+      <c r="L23" s="63"/>
+      <c r="M23" s="63"/>
+      <c r="N23" s="63"/>
+      <c r="O23" s="63"/>
+      <c r="P23" s="63"/>
+      <c r="Q23" s="63"/>
+      <c r="R23" s="64"/>
+    </row>
+    <row r="24" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="G24" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="H24" s="86" t="s">
+        <v>8</v>
+      </c>
+      <c r="I24" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="J24" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="K24" s="86" t="s">
+        <v>31</v>
+      </c>
+      <c r="L24" s="86" t="s">
+        <v>32</v>
+      </c>
+      <c r="M24" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="N24" s="86" t="s">
+        <v>34</v>
+      </c>
+      <c r="O24" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="P24" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q24" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="R24" s="23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="38">
+        <v>150</v>
+      </c>
+      <c r="E25" s="40">
+        <v>535</v>
+      </c>
+      <c r="F25" s="41">
+        <v>1</v>
+      </c>
+      <c r="G25" s="42">
+        <v>1</v>
+      </c>
+      <c r="H25" s="81">
+        <v>0</v>
+      </c>
+      <c r="I25" s="42">
+        <v>1</v>
+      </c>
+      <c r="J25" s="42">
+        <v>2</v>
+      </c>
+      <c r="K25" s="81">
+        <v>0</v>
+      </c>
+      <c r="L25" s="81">
+        <v>0</v>
+      </c>
+      <c r="M25" s="42">
+        <v>0</v>
+      </c>
+      <c r="N25" s="81">
+        <v>0</v>
+      </c>
+      <c r="O25" s="42">
+        <v>0</v>
+      </c>
+      <c r="P25" s="42">
+        <v>2</v>
+      </c>
+      <c r="Q25" s="43">
+        <v>1</v>
+      </c>
+      <c r="R25" s="24">
+        <f>(SUM(F25:Q25))</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="8">
+        <v>250</v>
+      </c>
+      <c r="E26" s="17">
+        <v>535</v>
+      </c>
+      <c r="F26" s="2">
+        <v>2</v>
+      </c>
+      <c r="G26" s="1">
+        <v>1</v>
+      </c>
+      <c r="H26" s="82">
+        <v>0</v>
+      </c>
+      <c r="I26" s="1">
+        <v>1</v>
+      </c>
+      <c r="J26" s="1">
+        <v>1</v>
+      </c>
+      <c r="K26" s="82">
+        <v>0</v>
+      </c>
+      <c r="L26" s="82">
+        <v>0</v>
+      </c>
+      <c r="M26" s="1">
+        <v>0</v>
+      </c>
+      <c r="N26" s="82">
+        <v>0</v>
+      </c>
+      <c r="O26" s="1">
+        <v>1</v>
+      </c>
+      <c r="P26" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="21">
+        <v>1</v>
+      </c>
+      <c r="R26" s="25">
+        <f t="shared" ref="R26:R32" si="3">(SUM(F26:Q26))</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="11">
+        <v>350</v>
+      </c>
+      <c r="E27" s="18">
+        <v>535</v>
+      </c>
+      <c r="F27" s="19">
+        <v>1</v>
+      </c>
+      <c r="G27" s="20">
+        <v>1</v>
+      </c>
+      <c r="H27" s="83">
+        <v>0</v>
+      </c>
+      <c r="I27" s="20">
+        <v>1</v>
+      </c>
+      <c r="J27" s="20">
+        <v>0</v>
+      </c>
+      <c r="K27" s="83">
+        <v>0</v>
+      </c>
+      <c r="L27" s="83">
+        <v>0</v>
+      </c>
+      <c r="M27" s="20">
+        <v>1</v>
+      </c>
+      <c r="N27" s="83">
+        <v>0</v>
+      </c>
+      <c r="O27" s="20">
+        <v>1</v>
+      </c>
+      <c r="P27" s="20">
+        <v>2</v>
+      </c>
+      <c r="Q27" s="22">
+        <v>0</v>
+      </c>
+      <c r="R27" s="26">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="55" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="56" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="57" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="56">
+        <v>150</v>
+      </c>
+      <c r="E28" s="58">
+        <v>535</v>
+      </c>
+      <c r="F28" s="88"/>
+      <c r="G28" s="84"/>
+      <c r="H28" s="84">
+        <v>0</v>
+      </c>
+      <c r="I28" s="84"/>
+      <c r="J28" s="84"/>
+      <c r="K28" s="84">
+        <v>0</v>
+      </c>
+      <c r="L28" s="84">
+        <v>0</v>
+      </c>
+      <c r="M28" s="84"/>
+      <c r="N28" s="84">
+        <v>0</v>
+      </c>
+      <c r="O28" s="84"/>
+      <c r="P28" s="84"/>
+      <c r="Q28" s="89"/>
+      <c r="R28" s="87"/>
+    </row>
+    <row r="29" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" s="49" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" s="48">
+        <v>250</v>
+      </c>
+      <c r="E29" s="50">
+        <v>535</v>
+      </c>
+      <c r="F29" s="90"/>
+      <c r="G29" s="85"/>
+      <c r="H29" s="85">
+        <v>0</v>
+      </c>
+      <c r="I29" s="85"/>
+      <c r="J29" s="85"/>
+      <c r="K29" s="85">
+        <v>0</v>
+      </c>
+      <c r="L29" s="85">
+        <v>0</v>
+      </c>
+      <c r="M29" s="85"/>
+      <c r="N29" s="85">
+        <v>0</v>
+      </c>
+      <c r="O29" s="85"/>
+      <c r="P29" s="85"/>
+      <c r="Q29" s="91"/>
+      <c r="R29" s="92"/>
+    </row>
+    <row r="30" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="D30" s="38">
+        <v>100</v>
+      </c>
+      <c r="E30" s="39">
+        <v>535</v>
+      </c>
+      <c r="F30" s="42">
+        <v>1</v>
+      </c>
+      <c r="G30" s="42">
+        <v>1</v>
+      </c>
+      <c r="H30" s="81">
+        <v>0</v>
+      </c>
+      <c r="I30" s="42">
+        <v>0</v>
+      </c>
+      <c r="J30" s="42">
+        <v>2</v>
+      </c>
+      <c r="K30" s="81">
+        <v>0</v>
+      </c>
+      <c r="L30" s="81">
+        <v>0</v>
+      </c>
+      <c r="M30" s="42">
+        <v>0</v>
+      </c>
+      <c r="N30" s="81">
+        <v>0</v>
+      </c>
+      <c r="O30" s="42">
+        <v>1</v>
+      </c>
+      <c r="P30" s="42">
+        <v>2</v>
+      </c>
+      <c r="Q30" s="43">
+        <v>0</v>
+      </c>
+      <c r="R30" s="24">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" s="8">
+        <v>150</v>
+      </c>
+      <c r="E31" s="9">
+        <v>535</v>
+      </c>
+      <c r="F31" s="1">
+        <v>1</v>
+      </c>
+      <c r="G31" s="1">
+        <v>1</v>
+      </c>
+      <c r="H31" s="82">
+        <v>0</v>
+      </c>
+      <c r="I31" s="1">
+        <v>1</v>
+      </c>
+      <c r="J31" s="1">
+        <v>2</v>
+      </c>
+      <c r="K31" s="82">
+        <v>0</v>
+      </c>
+      <c r="L31" s="82">
+        <v>0</v>
+      </c>
+      <c r="M31" s="1">
+        <v>1</v>
+      </c>
+      <c r="N31" s="82">
+        <v>0</v>
+      </c>
+      <c r="O31" s="1">
+        <v>1</v>
+      </c>
+      <c r="P31" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="21">
+        <v>0</v>
+      </c>
+      <c r="R31" s="25">
+        <f t="shared" ref="R31" si="4">(SUM(F31:Q31))</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D32" s="11">
+        <v>250</v>
+      </c>
+      <c r="E32" s="12">
+        <v>535</v>
+      </c>
+      <c r="F32" s="20">
+        <v>1</v>
+      </c>
+      <c r="G32" s="20">
+        <v>1</v>
+      </c>
+      <c r="H32" s="83">
+        <v>0</v>
+      </c>
+      <c r="I32" s="20">
+        <v>1</v>
+      </c>
+      <c r="J32" s="20">
+        <v>2</v>
+      </c>
+      <c r="K32" s="83">
+        <v>0</v>
+      </c>
+      <c r="L32" s="83">
+        <v>0</v>
+      </c>
+      <c r="M32" s="20">
+        <v>1</v>
+      </c>
+      <c r="N32" s="83">
+        <v>0</v>
+      </c>
+      <c r="O32" s="20">
+        <v>0</v>
+      </c>
+      <c r="P32" s="20">
+        <v>2</v>
+      </c>
+      <c r="Q32" s="20">
+        <v>1</v>
+      </c>
+      <c r="R32" s="26">
+        <f t="shared" ref="R32:R36" si="5">(SUM(F32:Q32))</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="71"/>
+      <c r="B33" s="71"/>
+      <c r="C33" s="71"/>
+      <c r="D33" s="71"/>
+      <c r="E33" s="71"/>
+      <c r="F33" s="72"/>
+      <c r="G33" s="73"/>
+      <c r="H33" s="73"/>
+      <c r="I33" s="73"/>
+      <c r="J33" s="73"/>
+      <c r="K33" s="73"/>
+      <c r="L33" s="73"/>
+      <c r="M33" s="73"/>
+      <c r="N33" s="73"/>
+      <c r="O33" s="73"/>
+      <c r="P33" s="71"/>
+      <c r="Q33" s="71"/>
+      <c r="R33" s="45">
+        <f>AVERAGE(R25:R32)</f>
+        <v>7.833333333333333</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="71"/>
+      <c r="B34" s="71"/>
+      <c r="C34" s="71"/>
+      <c r="D34" s="71"/>
+      <c r="E34" s="71"/>
+      <c r="F34" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="G34" s="63"/>
+      <c r="H34" s="63"/>
+      <c r="I34" s="63"/>
+      <c r="J34" s="63"/>
+      <c r="K34" s="63"/>
+      <c r="L34" s="63"/>
+      <c r="M34" s="63"/>
+      <c r="N34" s="63"/>
+      <c r="O34" s="63"/>
+      <c r="P34" s="63"/>
+      <c r="Q34" s="64"/>
+      <c r="R34" s="76"/>
+    </row>
+    <row r="35" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="71"/>
+      <c r="B35" s="71"/>
+      <c r="C35" s="71"/>
+      <c r="D35" s="71"/>
+      <c r="E35" s="71"/>
+      <c r="F35" s="27">
+        <f t="shared" ref="F35:Q35" si="6">AVERAGE(F25:F32)/2*100</f>
+        <v>58.333333333333336</v>
+      </c>
+      <c r="G35" s="27">
+        <f t="shared" si="6"/>
+        <v>50</v>
+      </c>
+      <c r="H35" s="87"/>
+      <c r="I35" s="27">
+        <f t="shared" si="6"/>
+        <v>41.666666666666671</v>
+      </c>
+      <c r="J35" s="27">
+        <f t="shared" si="6"/>
+        <v>75</v>
+      </c>
+      <c r="K35" s="87"/>
+      <c r="L35" s="87"/>
+      <c r="M35" s="27">
+        <f t="shared" si="6"/>
+        <v>25</v>
+      </c>
+      <c r="N35" s="87"/>
+      <c r="O35" s="27">
+        <f t="shared" si="6"/>
+        <v>33.333333333333329</v>
+      </c>
+      <c r="P35" s="27">
+        <f t="shared" si="6"/>
+        <v>83.333333333333343</v>
+      </c>
+      <c r="Q35" s="44">
+        <f t="shared" si="6"/>
+        <v>25</v>
+      </c>
+      <c r="R35" s="45">
+        <f>SUM(F35:Q35)</f>
+        <v>391.66666666666663</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="71"/>
+      <c r="B36" s="71"/>
+      <c r="C36" s="71"/>
+      <c r="D36" s="71"/>
+      <c r="E36" s="71"/>
+      <c r="F36" s="72"/>
+      <c r="G36" s="73"/>
+      <c r="H36" s="73"/>
+      <c r="I36" s="73"/>
+      <c r="J36" s="73"/>
+      <c r="K36" s="73"/>
+      <c r="L36" s="73"/>
+      <c r="M36" s="73"/>
+      <c r="N36" s="73"/>
+      <c r="O36" s="73"/>
+      <c r="P36" s="71"/>
+      <c r="Q36" s="71"/>
+      <c r="R36" s="45">
+        <f>AVERAGE(F35:Q35)</f>
+        <v>48.958333333333329</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P38" t="s">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="12">
+    <mergeCell ref="F34:Q34"/>
+    <mergeCell ref="F19:Q19"/>
+    <mergeCell ref="A1:E4"/>
+    <mergeCell ref="A19:E22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:R23"/>
     <mergeCell ref="F1:Q1"/>
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="D5:E5"/>
@@ -2078,7 +2938,7 @@
     <mergeCell ref="F16:Q16"/>
   </mergeCells>
   <conditionalFormatting sqref="F7:Q14">
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -2090,6 +2950,42 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R7:R14">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F17:Q17">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F25:G32 O25:Q32 M25:M32 I25:J32">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="2"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <color theme="7" tint="0.39997558519241921"/>
+        <color theme="9" tint="0.39997558519241921"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R25:R32">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2101,7 +2997,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F17:Q17">
+  <conditionalFormatting sqref="F35:Q35">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>